<commit_message>
ERD & Risk management
</commit_message>
<xml_diff>
--- a/Documentation/Risk Management.xlsx
+++ b/Documentation/Risk Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dharmindra.s.kaila\IndividualProject1\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F547F1-96C9-48E1-996F-3717192EF39D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0947256D-052A-43F8-A09A-505A06A251D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2508" yWindow="2184" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
   <si>
     <t>Description</t>
   </si>
@@ -66,13 +66,119 @@
     <t>Sean Kaila</t>
   </si>
   <si>
-    <t xml:space="preserve">Contimue development on my own laptop until a replacement arrives </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Make sure laptop is update and working correctly reggulary </t>
-  </si>
-  <si>
     <t xml:space="preserve">No updates at of 23/04/2021. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make sure laptop is update and working correctly regulary </t>
+  </si>
+  <si>
+    <t>Results in exposure of passwords 
+and other information to individuals who should not be able to see it</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>if the information where to reach the wrong had,
+ change the passwords and other informationassociated with data breach</t>
+  </si>
+  <si>
+    <t>Use a GitIgnore file to hide connection strings, 
+passwords and test result files from being pushed to github</t>
+  </si>
+  <si>
+    <t>No updates as of 08/05/2021</t>
+  </si>
+  <si>
+    <t>Key progress of project lost. Therefore 
+not able to deliver project deliverables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pull latest changes from the branch you're currently
+working on. </t>
+  </si>
+  <si>
+    <t>Make sure to regulary push and commit to git</t>
+  </si>
+  <si>
+    <t>Critial information pushed to github.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client will not have access to the 
+production environment. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continue development on my own laptop until a replacement arrives </t>
+  </si>
+  <si>
+    <t>Deploy project on a parallel app service until the problem is resolved.</t>
+  </si>
+  <si>
+    <t>Regularly check server status 
+and set up a notification services to let somone know when the service has stopped working.</t>
+  </si>
+  <si>
+    <t>Azure App Service Outage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loss of core data stops clients from 
+using app. </t>
+  </si>
+  <si>
+    <t>MySQL Database Faliure</t>
+  </si>
+  <si>
+    <t>Meduim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restore database from 
+a backup databse, so that clients go use app once again with minimal loss. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continue to back up Database twice a day
+(Every 12 hours.) </t>
+  </si>
+  <si>
+    <t>code Loss (Local)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit feature failing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Users not being able to use 
+cure functionality. </t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Investigate the issue as soon as 
+it arrives and deploy a hot fix.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continue to Test edit functionality
+making sure that its being tested correctly. </t>
+  </si>
+  <si>
+    <t>Scope Creep</t>
+  </si>
+  <si>
+    <t>Results in core areas being unpolished 
+due to the amunt of taks needed to be complete in a short space of time.</t>
+  </si>
+  <si>
+    <t>meduim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delay the release of the product, 
+allowing for core functionality to be more polished. </t>
+  </si>
+  <si>
+    <t>Revaluate the requirements against 
+what work is being done to minimuse the riskof spending too much time on unimportant tasks compered to the important ones.</t>
   </si>
 </sst>
 </file>
@@ -143,7 +249,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -515,25 +642,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H3"/>
+  <dimension ref="A2:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.90625" customWidth="1"/>
+    <col min="1" max="1" width="32.88671875" customWidth="1"/>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.81640625" customWidth="1"/>
-    <col min="4" max="4" width="20.54296875" customWidth="1"/>
-    <col min="5" max="5" width="20.08984375" customWidth="1"/>
+    <col min="3" max="3" width="28.77734375" customWidth="1"/>
+    <col min="4" max="4" width="20.5546875" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="21.7265625" customWidth="1"/>
-    <col min="8" max="8" width="29.26953125" customWidth="1"/>
+    <col min="7" max="7" width="21.77734375" customWidth="1"/>
+    <col min="8" max="8" width="29.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,7 +686,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -576,13 +703,169 @@
         <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Risk management and Use case diagram
</commit_message>
<xml_diff>
--- a/Documentation/Risk Management.xlsx
+++ b/Documentation/Risk Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dharmindra.s.kaila\IndividualProject1\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0947256D-052A-43F8-A09A-505A06A251D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8AC569-E850-4186-89F9-914454E24808}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2508" yWindow="2184" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
   <si>
     <t>Description</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Control Measures</t>
   </si>
   <si>
-    <t>Updates</t>
-  </si>
-  <si>
     <t xml:space="preserve">Laptop Faliure. </t>
   </si>
   <si>
@@ -67,9 +64,6 @@
   </si>
   <si>
     <t xml:space="preserve">No updates at of 23/04/2021. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Make sure laptop is update and working correctly regulary </t>
   </si>
   <si>
     <t>Results in exposure of passwords 
@@ -101,9 +95,6 @@
 working on. </t>
   </si>
   <si>
-    <t>Make sure to regulary push and commit to git</t>
-  </si>
-  <si>
     <t>Critial information pushed to github.</t>
   </si>
   <si>
@@ -117,10 +108,6 @@
     <t>Deploy project on a parallel app service until the problem is resolved.</t>
   </si>
   <si>
-    <t>Regularly check server status 
-and set up a notification services to let somone know when the service has stopped working.</t>
-  </si>
-  <si>
     <t>Azure App Service Outage.</t>
   </si>
   <si>
@@ -138,13 +125,6 @@
 a backup databse, so that clients go use app once again with minimal loss. </t>
   </si>
   <si>
-    <t xml:space="preserve">Continue to back up Database twice a day
-(Every 12 hours.) </t>
-  </si>
-  <si>
-    <t>code Loss (Local)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Edit feature failing </t>
   </si>
   <si>
@@ -177,15 +157,55 @@
 allowing for core functionality to be more polished. </t>
   </si>
   <si>
+    <t>Code Loss (Local)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regularly check server status 
+</t>
+  </si>
+  <si>
+    <t>Continue to back up Database at least once a day.</t>
+  </si>
+  <si>
     <t>Revaluate the requirements against 
-what work is being done to minimuse the riskof spending too much time on unimportant tasks compered to the important ones.</t>
+what work is being done to minimuse the risk of spending too much time on unimportant tasks compered to the important ones.</t>
+  </si>
+  <si>
+    <t>Office internet Outage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not able to continue development until
+another way of connection to the internet is established. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continue development on a hotspot 
+until normal access to the internet is established again. </t>
+  </si>
+  <si>
+    <t>No updates as of 09/05/2021</t>
+  </si>
+  <si>
+    <t>No updates as of 07/05/2021</t>
+  </si>
+  <si>
+    <t>Updates / Review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make sure laptop is update and working correctly regularly </t>
+  </si>
+  <si>
+    <t>Make sure to regularly push and commit to git</t>
+  </si>
+  <si>
+    <t>Always use an ethernet cable 
+to minimise the risk of wifi cutting out.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,13 +221,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -234,43 +290,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -642,25 +686,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H9"/>
+  <dimension ref="A2:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.88671875" customWidth="1"/>
+    <col min="1" max="1" width="32.90625" customWidth="1"/>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.77734375" customWidth="1"/>
-    <col min="4" max="4" width="20.5546875" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" customWidth="1"/>
+    <col min="3" max="3" width="28.81640625" customWidth="1"/>
+    <col min="4" max="4" width="20.54296875" customWidth="1"/>
+    <col min="5" max="5" width="20.08984375" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="21.77734375" customWidth="1"/>
-    <col min="8" max="8" width="29.21875" customWidth="1"/>
+    <col min="7" max="7" width="21.81640625" customWidth="1"/>
+    <col min="8" max="8" width="29.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -668,7 +712,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
@@ -683,189 +727,215 @@
         <v>5</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
+    <row r="4" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E6" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="F6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
+      <c r="C7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="4" t="s">
+    <row r="8" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
+      <c r="D9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="10" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H9" t="s">
-        <v>20</v>
+      <c r="G10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>